<commit_message>
Fix: Use tracking period data instead of natural days
- Correct today's count from 15 to 12 (matching XTracker)
- Use EST timezone for date grouping
- Query entire tracking period instead of single day

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/elon_musk_tweets.xlsx
+++ b/data/elon_musk_tweets.xlsx
@@ -519,7 +519,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="n">
-        <v>-43.1</v>
+        <v>-42.8</v>
       </c>
     </row>
     <row r="3">
@@ -543,7 +543,7 @@
         <v>35</v>
       </c>
       <c r="F3" t="n">
-        <v>-3.1</v>
+        <v>-2.8</v>
       </c>
     </row>
     <row r="4">
@@ -567,7 +567,7 @@
         <v>42.7</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5">
@@ -591,7 +591,7 @@
         <v>42.8</v>
       </c>
       <c r="F5" t="n">
-        <v>-15.1</v>
+        <v>-14.8</v>
       </c>
     </row>
     <row r="6">
@@ -615,7 +615,7 @@
         <v>38.4</v>
       </c>
       <c r="F6" t="n">
-        <v>-37.1</v>
+        <v>-36.8</v>
       </c>
     </row>
     <row r="7">
@@ -639,7 +639,7 @@
         <v>35.5</v>
       </c>
       <c r="F7" t="n">
-        <v>-37.1</v>
+        <v>-36.8</v>
       </c>
     </row>
     <row r="8">
@@ -663,7 +663,7 @@
         <v>34.4</v>
       </c>
       <c r="F8" t="n">
-        <v>-30.1</v>
+        <v>-29.8</v>
       </c>
     </row>
     <row r="9">
@@ -687,7 +687,7 @@
         <v>38.3</v>
       </c>
       <c r="F9" t="n">
-        <v>-16.1</v>
+        <v>-15.8</v>
       </c>
     </row>
     <row r="10">
@@ -711,7 +711,7 @@
         <v>34.9</v>
       </c>
       <c r="F10" t="n">
-        <v>-27.1</v>
+        <v>-26.8</v>
       </c>
     </row>
     <row r="11">
@@ -735,7 +735,7 @@
         <v>35.6</v>
       </c>
       <c r="F11" t="n">
-        <v>4.9</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="12">
@@ -759,7 +759,7 @@
         <v>33.3</v>
       </c>
       <c r="F12" t="n">
-        <v>-31.1</v>
+        <v>-30.8</v>
       </c>
     </row>
     <row r="13">
@@ -783,7 +783,7 @@
         <v>41.7</v>
       </c>
       <c r="F13" t="n">
-        <v>21.9</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="14">
@@ -807,7 +807,7 @@
         <v>40.1</v>
       </c>
       <c r="F14" t="n">
-        <v>-48.1</v>
+        <v>-47.8</v>
       </c>
     </row>
     <row r="15">
@@ -831,7 +831,7 @@
         <v>48.6</v>
       </c>
       <c r="F15" t="n">
-        <v>28.9</v>
+        <v>29.2</v>
       </c>
     </row>
     <row r="16">
@@ -855,7 +855,7 @@
         <v>49</v>
       </c>
       <c r="F16" t="n">
-        <v>-13.1</v>
+        <v>-12.8</v>
       </c>
     </row>
     <row r="17">
@@ -879,7 +879,7 @@
         <v>48.9</v>
       </c>
       <c r="F17" t="n">
-        <v>-28.1</v>
+        <v>-27.8</v>
       </c>
     </row>
     <row r="18">
@@ -903,7 +903,7 @@
         <v>50</v>
       </c>
       <c r="F18" t="n">
-        <v>12.9</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="19">
@@ -927,7 +927,7 @@
         <v>51.1</v>
       </c>
       <c r="F19" t="n">
-        <v>-23.1</v>
+        <v>-22.8</v>
       </c>
     </row>
     <row r="20">
@@ -951,7 +951,7 @@
         <v>47.3</v>
       </c>
       <c r="F20" t="n">
-        <v>-5.1</v>
+        <v>-4.8</v>
       </c>
     </row>
     <row r="21">
@@ -975,7 +975,7 @@
         <v>53.1</v>
       </c>
       <c r="F21" t="n">
-        <v>-7.1</v>
+        <v>-6.8</v>
       </c>
     </row>
     <row r="22">
@@ -999,7 +999,7 @@
         <v>48.4</v>
       </c>
       <c r="F22" t="n">
-        <v>-4.1</v>
+        <v>-3.8</v>
       </c>
     </row>
     <row r="23">
@@ -1023,7 +1023,7 @@
         <v>55.1</v>
       </c>
       <c r="F23" t="n">
-        <v>33.9</v>
+        <v>34.2</v>
       </c>
     </row>
     <row r="24">
@@ -1047,7 +1047,7 @@
         <v>65.40000000000001</v>
       </c>
       <c r="F24" t="n">
-        <v>43.9</v>
+        <v>44.2</v>
       </c>
     </row>
     <row r="25">
@@ -1071,7 +1071,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="n">
-        <v>30.9</v>
+        <v>31.2</v>
       </c>
     </row>
     <row r="26">
@@ -1095,7 +1095,7 @@
         <v>70.7</v>
       </c>
       <c r="F26" t="n">
-        <v>-4.1</v>
+        <v>-3.8</v>
       </c>
     </row>
     <row r="27">
@@ -1119,7 +1119,7 @@
         <v>72.3</v>
       </c>
       <c r="F27" t="n">
-        <v>5.9</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="28">
@@ -1143,7 +1143,7 @@
         <v>78.3</v>
       </c>
       <c r="F28" t="n">
-        <v>34.9</v>
+        <v>35.2</v>
       </c>
     </row>
     <row r="29">
@@ -1167,7 +1167,7 @@
         <v>82.59999999999999</v>
       </c>
       <c r="F29" t="n">
-        <v>25.9</v>
+        <v>26.2</v>
       </c>
     </row>
     <row r="30">
@@ -1191,7 +1191,7 @@
         <v>77.40000000000001</v>
       </c>
       <c r="F30" t="n">
-        <v>-2.1</v>
+        <v>-1.8</v>
       </c>
     </row>
     <row r="31">
@@ -1215,7 +1215,7 @@
         <v>73.40000000000001</v>
       </c>
       <c r="F31" t="n">
-        <v>15.9</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="32">
@@ -1239,7 +1239,7 @@
         <v>72.59999999999999</v>
       </c>
       <c r="F32" t="n">
-        <v>24.9</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="33">
@@ -1263,7 +1263,7 @@
         <v>80.40000000000001</v>
       </c>
       <c r="F33" t="n">
-        <v>50.9</v>
+        <v>51.2</v>
       </c>
     </row>
     <row r="34">
@@ -1287,7 +1287,7 @@
         <v>82</v>
       </c>
       <c r="F34" t="n">
-        <v>16.9</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="35">
@@ -1311,7 +1311,7 @@
         <v>84.40000000000001</v>
       </c>
       <c r="F35" t="n">
-        <v>51.9</v>
+        <v>52.2</v>
       </c>
     </row>
     <row r="36">
@@ -1335,7 +1335,7 @@
         <v>84.40000000000001</v>
       </c>
       <c r="F36" t="n">
-        <v>25.9</v>
+        <v>26.2</v>
       </c>
     </row>
     <row r="37">
@@ -1359,7 +1359,7 @@
         <v>81.7</v>
       </c>
       <c r="F37" t="n">
-        <v>-21.1</v>
+        <v>-20.8</v>
       </c>
     </row>
     <row r="38">
@@ -1383,7 +1383,7 @@
         <v>77.3</v>
       </c>
       <c r="F38" t="n">
-        <v>-15.1</v>
+        <v>-14.8</v>
       </c>
     </row>
     <row r="39">
@@ -1407,7 +1407,7 @@
         <v>79.7</v>
       </c>
       <c r="F39" t="n">
-        <v>41.9</v>
+        <v>42.2</v>
       </c>
     </row>
     <row r="40">
@@ -1431,7 +1431,7 @@
         <v>75.40000000000001</v>
       </c>
       <c r="F40" t="n">
-        <v>20.9</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="41">
@@ -1455,7 +1455,7 @@
         <v>82</v>
       </c>
       <c r="F41" t="n">
-        <v>62.9</v>
+        <v>63.2</v>
       </c>
     </row>
     <row r="42">
@@ -1479,7 +1479,7 @@
         <v>75.59999999999999</v>
       </c>
       <c r="F42" t="n">
-        <v>6.9</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="43">
@@ -1503,7 +1503,7 @@
         <v>73.3</v>
       </c>
       <c r="F43" t="n">
-        <v>9.9</v>
+        <v>10.2</v>
       </c>
     </row>
     <row r="44">
@@ -1527,7 +1527,7 @@
         <v>74.90000000000001</v>
       </c>
       <c r="F44" t="n">
-        <v>-10.1</v>
+        <v>-9.800000000000001</v>
       </c>
     </row>
     <row r="45">
@@ -1551,7 +1551,7 @@
         <v>76.90000000000001</v>
       </c>
       <c r="F45" t="n">
-        <v>-1.1</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="46">
@@ -1575,7 +1575,7 @@
         <v>65.90000000000001</v>
       </c>
       <c r="F46" t="n">
-        <v>-35.1</v>
+        <v>-34.8</v>
       </c>
     </row>
     <row r="47">
@@ -1599,7 +1599,7 @@
         <v>68.40000000000001</v>
       </c>
       <c r="F47" t="n">
-        <v>38.9</v>
+        <v>39.2</v>
       </c>
     </row>
     <row r="48">
@@ -1623,7 +1623,7 @@
         <v>62.9</v>
       </c>
       <c r="F48" t="n">
-        <v>23.9</v>
+        <v>24.2</v>
       </c>
     </row>
     <row r="49">
@@ -1647,7 +1647,7 @@
         <v>59.9</v>
       </c>
       <c r="F49" t="n">
-        <v>-14.1</v>
+        <v>-13.8</v>
       </c>
     </row>
     <row r="50">
@@ -1671,7 +1671,7 @@
         <v>58.7</v>
       </c>
       <c r="F50" t="n">
-        <v>1.9</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="51">
@@ -1695,7 +1695,7 @@
         <v>59</v>
       </c>
       <c r="F51" t="n">
-        <v>-8.1</v>
+        <v>-7.8</v>
       </c>
     </row>
     <row r="52">
@@ -1719,7 +1719,7 @@
         <v>56.4</v>
       </c>
       <c r="F52" t="n">
-        <v>-19.1</v>
+        <v>-18.8</v>
       </c>
     </row>
     <row r="53">
@@ -1743,7 +1743,7 @@
         <v>58.9</v>
       </c>
       <c r="F53" t="n">
-        <v>-18.1</v>
+        <v>-17.8</v>
       </c>
     </row>
     <row r="54">
@@ -1767,7 +1767,7 @@
         <v>58.9</v>
       </c>
       <c r="F54" t="n">
-        <v>38.9</v>
+        <v>39.2</v>
       </c>
     </row>
     <row r="55">
@@ -1791,7 +1791,7 @@
         <v>55.1</v>
       </c>
       <c r="F55" t="n">
-        <v>-2.1</v>
+        <v>-1.8</v>
       </c>
     </row>
     <row r="56">
@@ -1815,7 +1815,7 @@
         <v>55.1</v>
       </c>
       <c r="F56" s="3" t="n">
-        <v>-14.1</v>
+        <v>-13.8</v>
       </c>
     </row>
     <row r="57">
@@ -1839,7 +1839,7 @@
         <v>52.7</v>
       </c>
       <c r="F57" s="3" t="n">
-        <v>-15.1</v>
+        <v>-14.8</v>
       </c>
     </row>
     <row r="58">
@@ -1863,7 +1863,7 @@
         <v>50.4</v>
       </c>
       <c r="F58" s="3" t="n">
-        <v>-24.1</v>
+        <v>-23.8</v>
       </c>
     </row>
     <row r="59">
@@ -1873,7 +1873,7 @@
         </is>
       </c>
       <c r="B59" s="3" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
@@ -1884,10 +1884,10 @@
         <v>6</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>53.3</v>
+        <v>49.6</v>
       </c>
       <c r="F59" s="3" t="n">
-        <v>0.9</v>
+        <v>-24.8</v>
       </c>
     </row>
     <row r="60">
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="B60" s="3" t="n">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
@@ -1908,10 +1908,10 @@
         <v>6</v>
       </c>
       <c r="E60" s="3" t="n">
-        <v>53.4</v>
+        <v>51.1</v>
       </c>
       <c r="F60" s="3" t="n">
-        <v>-17.1</v>
+        <v>-6.8</v>
       </c>
     </row>
     <row r="61">
@@ -1921,7 +1921,7 @@
         </is>
       </c>
       <c r="B61" s="3" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
@@ -1932,10 +1932,10 @@
         <v>6</v>
       </c>
       <c r="E61" s="3" t="n">
-        <v>42.7</v>
+        <v>38.9</v>
       </c>
       <c r="F61" s="3" t="n">
-        <v>-36.1</v>
+        <v>-46.8</v>
       </c>
     </row>
     <row r="62">
@@ -1945,7 +1945,7 @@
         </is>
       </c>
       <c r="B62" s="3" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
@@ -1956,10 +1956,10 @@
         <v>6</v>
       </c>
       <c r="E62" s="3" t="n">
-        <v>35.4</v>
+        <v>33</v>
       </c>
       <c r="F62" s="3" t="n">
-        <v>-53.1</v>
+        <v>-42.8</v>
       </c>
     </row>
   </sheetData>
@@ -2014,7 +2014,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3543</v>
+        <v>3526</v>
       </c>
     </row>
     <row r="4">
@@ -2025,7 +2025,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>58.1</t>
+          <t>57.8</t>
         </is>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>55.0</t>
+          <t>54.0</t>
         </is>
       </c>
     </row>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>27.2</t>
+          <t>27.3</t>
         </is>
       </c>
     </row>
@@ -2093,7 +2093,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2026-02-06 16:29:17</t>
+          <t>2026-02-06 20:08:36</t>
         </is>
       </c>
     </row>
@@ -2233,16 +2233,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C7" t="n">
-        <v>32.2</v>
+        <v>28.8</v>
       </c>
       <c r="D7" t="n">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">

</xml_diff>